<commit_message>
update simulated and template database
</commit_message>
<xml_diff>
--- a/src/ALSTracker/doc/other/database_template.xlsx
+++ b/src/ALSTracker/doc/other/database_template.xlsx
@@ -5,16 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Phases" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="ALSFRS-R Score" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Vital capacity" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="Neurofilament light chain" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="Left-Hand Grip" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="Right-Hand Grip" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="Other" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Phases" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="ALSFRS-R Score" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Vital capacity" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Neurofilament light chain" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Left-Hand Grip" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="Right-Hand Grip" sheetId="8" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -95,6 +96,12 @@
   </si>
   <si>
     <t xml:space="preserve">RMAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onset</t>
   </si>
   <si>
     <t xml:space="preserve">Phasename</t>
@@ -188,12 +195,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -391,116 +402,116 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -516,6 +527,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -528,20 +576,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -555,7 +603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -568,15 +616,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -591,7 +639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -605,10 +653,10 @@
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -623,7 +671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -637,10 +685,10 @@
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -651,38 +699,6 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -700,11 +716,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>